<commit_message>
new fad data and working on saba/eustatia issue
</commit_message>
<xml_diff>
--- a/raw_data/fad_data/fad_numbers.xlsx
+++ b/raw_data/fad_data/fad_numbers.xlsx
@@ -1,27 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/fad_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F6E53-AD2A-3047-9AA7-AED27E69A9FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
+    <workbookView xWindow="11940" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fads_timeline" sheetId="6" r:id="rId1"/>
     <sheet name="fads_current" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" iterate="1" iterateCount="10" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,17 +27,20 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Molly Wilson</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="209">
   <si>
     <t>Anguilla</t>
   </si>
@@ -689,13 +690,28 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Theophile PC 2019</t>
+  </si>
+  <si>
+    <t>Meijer zu Schlochtern PC 2019</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Bart PC 2019; Frame survey</t>
+  </si>
+  <si>
+    <t>238 (2016)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -745,6 +761,12 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -775,7 +797,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -786,12 +808,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1170,21 +1193,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="9" max="9" width="22.5" customWidth="1"/>
     <col min="11" max="11" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>177</v>
       </c>
@@ -1219,7 +1242,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1307,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1340,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1350,7 +1373,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1383,7 +1406,7 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1418,7 +1441,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1470,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1473,7 +1496,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1481,7 +1504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1513,7 +1536,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1569,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1575,7 +1598,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -1607,7 +1630,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1637,7 +1660,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
@@ -1666,7 +1689,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1689,7 +1712,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1715,7 +1738,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1761,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1764,7 +1787,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -1796,7 +1819,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1826,7 +1849,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -1851,7 +1874,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11">
       <c r="A24" s="3" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1904,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1913,7 +1936,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1945,7 +1968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1997,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -2009,7 +2032,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -2038,7 +2061,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2067,7 +2090,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2096,7 +2119,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2148,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2154,7 +2177,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2189,7 +2212,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2222,7 +2245,7 @@
       </c>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2251,7 +2274,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2283,7 +2306,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2338,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -2344,7 +2367,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -2373,7 +2396,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2405,7 +2428,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2454,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -2463,7 +2486,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2495,7 +2518,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2527,7 +2550,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -2535,7 +2558,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2564,7 +2587,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2593,7 +2616,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2622,7 +2645,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2651,7 +2674,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2674,7 +2697,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2706,7 +2729,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2735,7 +2758,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2767,7 +2790,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2793,7 +2816,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2816,7 +2839,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2839,7 +2862,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -2868,7 +2891,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -2890,7 +2913,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -2916,7 +2939,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -2945,7 +2968,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2975,7 +2998,7 @@
       </c>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -3005,7 +3028,7 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -3035,7 +3058,7 @@
       </c>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:11">
       <c r="A65" s="1" t="s">
         <v>51</v>
       </c>
@@ -3064,7 +3087,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:11">
       <c r="A66" s="1" t="s">
         <v>51</v>
       </c>
@@ -3090,7 +3113,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:11">
       <c r="A67" s="1" t="s">
         <v>45</v>
       </c>
@@ -3119,7 +3142,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:11">
       <c r="A68" s="1" t="s">
         <v>52</v>
       </c>
@@ -3148,7 +3171,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:11">
       <c r="A69" s="1" t="s">
         <v>52</v>
       </c>
@@ -3181,7 +3204,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:11">
       <c r="A70" s="1" t="s">
         <v>52</v>
       </c>
@@ -3214,7 +3237,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:11">
       <c r="A71" s="3" t="s">
         <v>52</v>
       </c>
@@ -3249,7 +3272,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -3281,7 +3304,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -3313,7 +3336,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -3345,7 +3368,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -3377,7 +3400,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -3409,7 +3432,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3436,7 +3459,7 @@
       </c>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
         <v>164</v>
       </c>
@@ -3468,7 +3491,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3500,7 +3523,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -3529,7 +3552,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -3549,7 +3572,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -3572,7 +3595,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -3598,7 +3621,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:11">
       <c r="A84" s="1" t="s">
         <v>50</v>
       </c>
@@ -3621,7 +3644,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:11">
       <c r="A85" s="1" t="s">
         <v>50</v>
       </c>
@@ -3644,7 +3667,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:11">
       <c r="A86" s="1" t="s">
         <v>50</v>
       </c>
@@ -3670,7 +3693,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>165</v>
       </c>
@@ -3684,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:11">
       <c r="A88" s="3" t="s">
         <v>189</v>
       </c>
@@ -3713,7 +3736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:11">
       <c r="A89" s="3" t="s">
         <v>189</v>
       </c>
@@ -3739,7 +3762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:11">
       <c r="A90" s="3" t="s">
         <v>189</v>
       </c>
@@ -3768,7 +3791,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:11">
       <c r="A91" s="3" t="s">
         <v>189</v>
       </c>
@@ -3800,7 +3823,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:11">
       <c r="A92" s="3" t="s">
         <v>189</v>
       </c>
@@ -3829,7 +3852,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -3837,7 +3860,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>166</v>
       </c>
@@ -3845,7 +3868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>167</v>
       </c>
@@ -3874,7 +3897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>167</v>
       </c>
@@ -3903,7 +3926,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>167</v>
       </c>
@@ -3935,7 +3958,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>167</v>
       </c>
@@ -3962,7 +3985,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K98">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K98">
     <sortCondition ref="A2:A98"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -3972,16 +3995,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="I24:J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>177</v>
       </c>
@@ -4013,31 +4036,23 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7">
-        <v>25</v>
-      </c>
+      <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7">
-        <v>2019</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -4069,7 +4084,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4098,7 +4113,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -4114,7 +4129,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -4134,7 +4149,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -4166,7 +4181,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -4198,7 +4213,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -4233,7 +4248,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
@@ -4243,21 +4258,29 @@
       <c r="C10" s="7">
         <v>0</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="H10" s="7">
-        <v>2018</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+        <v>2019</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -4277,7 +4300,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>201</v>
@@ -4286,7 +4309,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -4294,7 +4317,7 @@
         <v>44</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>20</v>
@@ -4302,17 +4325,20 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="H12">
         <v>2019</v>
       </c>
-      <c r="I12" t="s">
-        <v>187</v>
+      <c r="I12" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="J12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -4322,11 +4348,20 @@
       <c r="C13">
         <v>40</v>
       </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>275</v>
+      </c>
       <c r="G13">
-        <v>434</v>
+        <v>325</v>
       </c>
       <c r="H13">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="I13" t="s">
         <v>195</v>
@@ -4335,7 +4370,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -4358,7 +4393,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -4390,7 +4425,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -4416,13 +4451,13 @@
         <v>2019</v>
       </c>
       <c r="I16" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="J16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -4432,6 +4467,12 @@
       <c r="C17">
         <v>18</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G17">
         <v>10700</v>
       </c>
@@ -4445,7 +4486,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -4465,7 +4506,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4500,7 +4541,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -4529,7 +4570,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4559,7 +4600,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -4591,7 +4632,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
@@ -4620,7 +4661,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -4652,7 +4693,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>164</v>
       </c>
@@ -4660,7 +4701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -4692,15 +4733,39 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>165</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>2019</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="3" t="s">
         <v>189</v>
       </c>
@@ -4732,7 +4797,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11">
       <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
@@ -4752,7 +4817,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11">
       <c r="A30" s="3" t="s">
         <v>166</v>
       </c>
@@ -4760,7 +4825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
syncing updated fad numbers
</commit_message>
<xml_diff>
--- a/raw_data/fad_data/fad_numbers.xlsx
+++ b/raw_data/fad_data/fad_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/github/kuni_fads/raw_data/fad_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gizmo/Github/kuni_fads/raw_data/fad_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B6ED9E6-4F72-5649-B50C-1765AC0F727F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBBC6C6-B500-3942-8F68-15D46E226D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="460" windowWidth="17760" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17760" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fads_timeline" sheetId="6" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="224">
   <si>
     <t>Anguilla</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>Deleveaux 2020</t>
+  </si>
+  <si>
+    <t>&gt;0</t>
   </si>
 </sst>
 </file>
@@ -4634,7 +4637,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5453,12 +5456,12 @@
       <c r="D22" s="17">
         <v>1</v>
       </c>
-      <c r="E22" s="17">
-        <v>0</v>
-      </c>
-      <c r="F22" s="16">
+      <c r="E22" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="F22" s="16" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G22" s="17">
         <v>158</v>
@@ -5799,12 +5802,12 @@
       <c r="D32" s="17">
         <v>4</v>
       </c>
-      <c r="E32" s="17">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16">
+      <c r="E32" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="16" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G32" s="17">
         <v>20</v>

</xml_diff>